<commit_message>
Update input file and template file
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t xml:space="preserve">Chairman</t>
   </si>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">MB</t>
   </si>
   <si>
+    <t xml:space="preserve">KT</t>
+  </si>
+  <si>
     <t xml:space="preserve">GJ</t>
   </si>
   <si>
@@ -68,43 +71,34 @@
     <t xml:space="preserve">GT</t>
   </si>
   <si>
+    <t xml:space="preserve">TF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CT</t>
+  </si>
+  <si>
     <t xml:space="preserve">SS</t>
   </si>
   <si>
-    <t xml:space="preserve">KT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP</t>
-  </si>
-  <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">EN</t>
   </si>
   <si>
-    <t xml:space="preserve">TF</t>
-  </si>
-  <si>
     <t xml:space="preserve">SF</t>
   </si>
   <si>
-    <t xml:space="preserve">SR</t>
-  </si>
-  <si>
     <t xml:space="preserve">JK</t>
   </si>
   <si>
     <t xml:space="preserve">CS</t>
   </si>
   <si>
-    <t xml:space="preserve">JB</t>
+    <t xml:space="preserve">JN</t>
   </si>
 </sst>
 </file>
@@ -115,7 +109,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-809]DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,6 +142,11 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -217,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +239,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -321,18 +324,16 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="13.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -361,7 +362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -372,16 +373,16 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>10</v>
@@ -390,33 +391,33 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -425,11 +426,11 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
@@ -438,7 +439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -449,53 +450,51 @@
         <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -503,86 +502,82 @@
         <v>18</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+    <row r="9" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -590,11 +585,9 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -602,9 +595,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="H14" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed multiple bugs in the Meeting Part Class
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Input List" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">'Input List'!$F$1:$F$1</definedName>
-    <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">'Input List'!$F$1:$F$1</definedName>
+    <definedName function="false" hidden="false" name="HTML_all" vbProcedure="false">'Input List'!$G$1:$G$1</definedName>
+    <definedName function="false" hidden="false" name="HTML_tables" vbProcedure="false">'Input List'!$G$1:$G$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">Chairman</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">Chairman Tue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chairman Fri</t>
   </si>
   <si>
     <t xml:space="preserve">Treasures 1</t>
@@ -109,7 +112,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-809]DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -142,11 +145,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="7.5"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -216,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,10 +237,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -322,13 +316,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="13.75"/>
   </cols>
@@ -358,19 +352,22 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -379,182 +376,209 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="5" t="n">
         <v>43595</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>20</v>
+      <c r="I7" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="I8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -566,6 +590,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
@@ -576,6 +601,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
@@ -586,6 +612,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
@@ -596,6 +623,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>